<commit_message>
alterado estrutura do jinja para adicionar instrumentos e vocais disponiveis e também mais colunas na tabela e validação de todas as colunas
</commit_message>
<xml_diff>
--- a/pessoas.xlsx
+++ b/pessoas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="52">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -28,9 +28,15 @@
     <t xml:space="preserve">Instrumentista</t>
   </si>
   <si>
+    <t xml:space="preserve">Instrumento</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vocalista</t>
   </si>
   <si>
+    <t xml:space="preserve">Tipo Vocal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Faz mensagem musical</t>
   </si>
   <si>
@@ -52,6 +58,9 @@
     <t xml:space="preserve">Sim</t>
   </si>
   <si>
+    <t xml:space="preserve">Tenor</t>
+  </si>
+  <si>
     <t xml:space="preserve">sabado</t>
   </si>
   <si>
@@ -73,6 +82,9 @@
     <t xml:space="preserve">Gabriel Vidal</t>
   </si>
   <si>
+    <t xml:space="preserve">Violão</t>
+  </si>
+  <si>
     <t xml:space="preserve">Davi Batista</t>
   </si>
   <si>
@@ -94,6 +106,9 @@
     <t xml:space="preserve">Michele</t>
   </si>
   <si>
+    <t xml:space="preserve">Baritono</t>
+  </si>
+  <si>
     <t xml:space="preserve">Matheus nascimento</t>
   </si>
   <si>
@@ -143,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">Jussara</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contralto</t>
   </si>
   <si>
     <t xml:space="preserve">Lucas</t>
@@ -262,20 +280,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J30" activeCellId="0" sqref="J30"/>
+      <selection pane="topLeft" activeCell="J31" activeCellId="0" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="23.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="10.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,487 +321,598 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>9</v>
+        <v>26</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q10" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>9</v>
+      <c r="I14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>9</v>
+        <v>35</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>9</v>
+        <v>37</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>9</v>
+        <v>39</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>9</v>
+      <c r="I25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>11</v>
+        <v>45</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>9</v>
+        <v>49</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>9</v>
+        <v>51</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>